<commit_message>
impl user cart(v1) 20251111_jkk
</commit_message>
<xml_diff>
--- a/스프링부트 미니프로젝트_prontend_v20251107.xlsx
+++ b/스프링부트 미니프로젝트_prontend_v20251107.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name=" API" sheetId="1" r:id="rId1"/>
     <sheet name="ProntEnd" sheetId="2" r:id="rId2"/>
+    <sheet name="요구사항 정리" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="201">
   <si>
     <t>공통 API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -557,12 +559,244 @@
     <t>관리자파트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>마이페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인페이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품상세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장바구니</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품제거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송정보입력(옵션)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결제하기(주문결제)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선택상품주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체상품주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자로그인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송지삭제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문배송관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문취소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원/로그인</t>
+  </si>
+  <si>
+    <t>회원가입 기능</t>
+  </si>
+  <si>
+    <t>로그인 기능</t>
+  </si>
+  <si>
+    <t>관리자 계정으로 로그인 하면 관리 사이트로 넘어간다.</t>
+  </si>
+  <si>
+    <t>상품/농작물 등록·관리</t>
+  </si>
+  <si>
+    <t>농작물 추가 기능</t>
+  </si>
+  <si>
+    <t>농작물 삭제 기능</t>
+  </si>
+  <si>
+    <t>농작물 재배 활성화/비활성화 기능</t>
+  </si>
+  <si>
+    <t>상품 등록 및 관리</t>
+  </si>
+  <si>
+    <t>창고에 있는 만큼의 농작물을 등록할 수 있다.</t>
+  </si>
+  <si>
+    <t>등록되어 있는 농작물은 게시를 중단할 수 있다.</t>
+  </si>
+  <si>
+    <t>검색/탐색</t>
+  </si>
+  <si>
+    <t>상품 검색 기능 (수확시기 등으로 필터 적용)</t>
+  </si>
+  <si>
+    <t>판매 사이트에 올라와 있는 농작물을 볼 수 있다.</t>
+  </si>
+  <si>
+    <t>장바구니/주문·결제</t>
+  </si>
+  <si>
+    <t>상품 구매 기능</t>
+  </si>
+  <si>
+    <t>상품 장바구니 기능</t>
+  </si>
+  <si>
+    <t>농작물의 페이지로 들어가 개수를 지정해서 장바구니에 담을 수 있다.</t>
+  </si>
+  <si>
+    <t>장바구니에 있는 농작물의 일부 혹은 전부 구매할 수 있다.</t>
+  </si>
+  <si>
+    <t>주문 조회/처리 - (관리자)</t>
+  </si>
+  <si>
+    <t>소비자가 주문한 농작물 조회 기능</t>
+  </si>
+  <si>
+    <t>주문 상태 변경 기능 → 배송 중으로 변경</t>
+  </si>
+  <si>
+    <t>배송 처리(주문 상품별 송장 번호 및 택배사 정보 입력)</t>
+  </si>
+  <si>
+    <t>주문 조회/처리(취소) - (사용자)</t>
+  </si>
+  <si>
+    <t>소비자가 주문한 주문 내역 조회 기능</t>
+  </si>
+  <si>
+    <t>재고/노출 관리 - (사용자)</t>
+  </si>
+  <si>
+    <t>통계/정산 - (관리자)</t>
+  </si>
+  <si>
+    <t>농작물 주문 통계 기능 (일자별/품목별 판매시 cnt++)</t>
+  </si>
+  <si>
+    <t>관리자</t>
+  </si>
+  <si>
+    <t>정산(판매 내역, 금액 조회)</t>
+  </si>
+  <si>
+    <t>계정/주소·계좌 관리</t>
+  </si>
+  <si>
+    <t>사용자</t>
+  </si>
+  <si>
+    <t>농가 정보, 계좌 등록</t>
+  </si>
+  <si>
+    <t>물품 상태가 배송 중으로 바뀌기 전에는 주문을 취소할 수 있다.</t>
+  </si>
+  <si>
+    <t>요구 사항 정리</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (품절 표기는 재고/노출과 연관, 배송 맥락과 함께 노출되는 문구로 함께 묶음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 사용자는 판매 페이지에서 재고가 없는 농작물은 자동으로 sold out 처리된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>●</t>
+  </si>
+  <si>
+    <t>●</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>☞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,8 +874,17 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="50"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,8 +909,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -719,13 +968,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -782,6 +1111,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,7 +1486,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1119,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1665,10 +2042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:O3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N34" sqref="A12:O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1678,10 +2055,14 @@
     <col min="3" max="3" width="51.375" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="6"/>
     <col min="6" max="6" width="11.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="6"/>
+    <col min="7" max="7" width="9" style="6"/>
+    <col min="8" max="8" width="18.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="9" style="6"/>
+    <col min="18" max="18" width="13" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>78</v>
       </c>
@@ -1700,7 +2081,7 @@
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -1717,7 +2098,7 @@
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -1734,7 +2115,7 @@
       <c r="N3" s="14"/>
       <c r="O3" s="14"/>
     </row>
-    <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>79</v>
       </c>
@@ -1742,7 +2123,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>73</v>
       </c>
@@ -1762,7 +2143,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>81</v>
       </c>
@@ -1779,7 +2160,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>122</v>
       </c>
@@ -1794,7 +2175,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>67</v>
       </c>
@@ -1806,7 +2187,7 @@
       </c>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>69</v>
       </c>
@@ -1818,7 +2199,7 @@
       </c>
       <c r="D10" s="18"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>132</v>
       </c>
@@ -1837,7 +2218,7 @@
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1854,7 +2235,7 @@
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1871,12 +2252,12 @@
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
     </row>
-    <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>64</v>
       </c>
@@ -1889,8 +2270,18 @@
       <c r="D16" s="7" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="R16" s="19"/>
+      <c r="S16" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>83</v>
       </c>
@@ -1903,8 +2294,20 @@
       <c r="D17" s="18" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>85</v>
       </c>
@@ -1915,8 +2318,11 @@
         <v>88</v>
       </c>
       <c r="D18" s="18"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S18" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1927,8 +2333,14 @@
         <v>82</v>
       </c>
       <c r="D19" s="18"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="S19" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>89</v>
       </c>
@@ -1939,8 +2351,11 @@
         <v>115</v>
       </c>
       <c r="D20" s="18"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S20" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>90</v>
       </c>
@@ -1951,8 +2366,11 @@
         <v>95</v>
       </c>
       <c r="D21" s="18"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S21" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>91</v>
       </c>
@@ -1963,8 +2381,11 @@
         <v>92</v>
       </c>
       <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S22" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>93</v>
       </c>
@@ -1975,8 +2396,19 @@
         <v>94</v>
       </c>
       <c r="D23" s="18"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q23" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="S23" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S24" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
         <v>133</v>
       </c>
@@ -1994,8 +2426,14 @@
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
       <c r="O25" s="14"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q25" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="S25" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -2011,8 +2449,11 @@
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S26" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -2028,13 +2469,25 @@
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
-    </row>
-    <row r="28" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+      <c r="Q27" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="S27" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="Q28" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="S28" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>64</v>
       </c>
@@ -2047,8 +2500,11 @@
       <c r="D29" s="7" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S29" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>96</v>
       </c>
@@ -2061,8 +2517,11 @@
       <c r="D30" s="18" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="S30" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>99</v>
       </c>
@@ -2073,8 +2532,14 @@
         <v>101</v>
       </c>
       <c r="D31" s="18"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="R31" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>102</v>
       </c>
@@ -2085,6 +2550,9 @@
         <v>104</v>
       </c>
       <c r="D32" s="18"/>
+      <c r="S32" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
@@ -2111,7 +2579,8 @@
       <c r="D34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="Q16:R16"/>
     <mergeCell ref="D30:D34"/>
     <mergeCell ref="A12:O14"/>
     <mergeCell ref="A1:O3"/>
@@ -2123,4 +2592,745 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:X28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:24" ht="72" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="24"/>
+    </row>
+    <row r="5" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="D5" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="O5" s="26" t="s">
+        <v>180</v>
+      </c>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="28"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D6" s="25"/>
+      <c r="E6" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P6" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="28"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D7" s="25"/>
+      <c r="E7" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="27"/>
+      <c r="W7" s="28"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D8" s="25"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="28"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="28"/>
+    </row>
+    <row r="10" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="D10" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="27"/>
+      <c r="V10" s="27"/>
+      <c r="W10" s="28"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D11" s="25"/>
+      <c r="E11" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P11" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="27"/>
+      <c r="W11" s="28"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D12" s="25"/>
+      <c r="E12" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="28"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D13" s="25"/>
+      <c r="E13" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="28"/>
+    </row>
+    <row r="14" spans="2:24" ht="24" x14ac:dyDescent="0.3">
+      <c r="D14" s="25"/>
+      <c r="E14" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="O14" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
+      <c r="W14" s="28"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D15" s="25"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P15" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
+      <c r="W15" s="28"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="D16" s="25"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="28"/>
+    </row>
+    <row r="17" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D17" s="25"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="28"/>
+    </row>
+    <row r="18" spans="4:23" ht="24" x14ac:dyDescent="0.3">
+      <c r="D18" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="O18" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="27"/>
+      <c r="W18" s="28"/>
+    </row>
+    <row r="19" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D19" s="25"/>
+      <c r="E19" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="27"/>
+      <c r="W19" s="28"/>
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D20" s="25"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="28"/>
+    </row>
+    <row r="21" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D21" s="25"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P21" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="27"/>
+      <c r="W21" s="28"/>
+    </row>
+    <row r="22" spans="4:23" ht="24" x14ac:dyDescent="0.3">
+      <c r="D22" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+      <c r="P22" s="27"/>
+      <c r="Q22" s="27"/>
+      <c r="R22" s="27"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="27"/>
+      <c r="W22" s="28"/>
+    </row>
+    <row r="23" spans="4:23" ht="24" x14ac:dyDescent="0.3">
+      <c r="D23" s="25"/>
+      <c r="E23" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="27"/>
+      <c r="N23" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="O23" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="P23" s="27"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="27"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="27"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="27"/>
+      <c r="W23" s="28"/>
+    </row>
+    <row r="24" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D24" s="25"/>
+      <c r="E24" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="W24" s="28"/>
+    </row>
+    <row r="25" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D25" s="25"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="27"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P25" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="27"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="27"/>
+      <c r="W25" s="28"/>
+    </row>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D26" s="25"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27"/>
+      <c r="U26" s="27"/>
+      <c r="V26" s="27"/>
+      <c r="W26" s="28"/>
+    </row>
+    <row r="27" spans="4:23" x14ac:dyDescent="0.3">
+      <c r="D27" s="25"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
+      <c r="M27" s="27"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="P27" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q27" s="27"/>
+      <c r="R27" s="27"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27"/>
+      <c r="U27" s="27"/>
+      <c r="V27" s="27"/>
+      <c r="W27" s="28"/>
+    </row>
+    <row r="28" spans="4:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="30"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="30"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="30"/>
+      <c r="W28" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:X3"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>